<commit_message>
import Purchases in crud.py
</commit_message>
<xml_diff>
--- a/app/parser/zakupki_44.xlsx
+++ b/app/parser/zakupki_44.xlsx
@@ -473,212 +473,212 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>№ 0330300016625000092</t>
+          <t>№ 0330300051225000216</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ СТАНЦИЯ СКОРОЙ МЕДИЦИНСКОЙ ПОМОЩИ" ИМЕНИ Н.Л. ТУРУПАНОВА</t>
+          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "ЦЕНТРАЛИЗОВАННАЯ БУХГАЛТЕРИЯ, ОБСЛУЖИВАЮЩАЯ МУНИЦИПАЛЬНЫЕ УЧРЕЖДЕНИЯ ГОРОДА ВОЛОГДЫ"</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Поставка запасных частей для автомобилей (Генераторы)</t>
+          <t>Оказание услуг по открытию возобновляемой кредитной линии в кредитной организации с лимитом задолженности в размере 300 000 000 (Триста миллионов) рублей в рамках исполнения бюджета города Вологды</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>323 250,00 ₽</t>
+          <t>60 510 000,00 ₽</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 27.11.2025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>44-ФЗ Запрос котировок в электронной форме</t>
+          <t>44-ФЗ Электронный аукцион</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300016625000092</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0330300051225000216</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>№ 0130600031225000390</t>
+          <t>№ 0330200021625000043</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>АДМИНИСТРАЦИЯ ВЕЛИКОУСТЮГСКОГО МУНИЦИПАЛЬНОГО ОКРУГА ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ КОЖНО-ВЕНЕРОЛОГИЧЕСКИЙ ДИСПАНСЕР № 2"</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Поставка средств индивидуальной защиты (респираторы и защитные очки)</t>
+          <t>Оказание услуг по сопровождению Электронного периодического справочника «Система ГАРАНТ» (информационного продукта вычислительной техники) (далее — ЭПС «Система ГАРАНТ»), содержащей информацию о текущем состоянии законодательства Российской Федерации, путем предоставления в электронном виде по каналам связи посредством телекоммуникационной сети Интернет формируемых текущих версий специальных информационных массивов (далее — СИМ) ЭПС «Система ГАРАНТ»</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>53 789,67 ₽</t>
+          <t>125 760,00 ₽</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0130600031225000390</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200021625000043</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>№ 0830500000225004196</t>
+          <t>№ 0330300002625000201</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ДЕТСКАЯ БОЛЬНИЦА № 2"</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Оказание услуг междугородной и международной телефонной связи</t>
+          <t>Оказание услуг по изготовлению и поставке экстемпоральных форм лекарственных препаратов (растворы)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1 033 000,00 ₽</t>
+          <t>492 700,00 ₽</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>05.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004196</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300002625000201</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>№ 0830500000225003923</t>
+          <t>№ 0330300034525000086</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "КАДУЙСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Поставка продуктов питания</t>
+          <t>Поставка медицинских изделий (Спирометр диагностический), ввод в эксплуатацию медицинских изделий, обучение правилам эксплуатации специалистов, эксплуатирующих медицинские изделия</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>720 847,00 ₽</t>
+          <t>465 000,00 ₽</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>20.10.2025, 17.11.2025, 07.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>44-ФЗ Открытый конкурс в электронной форме</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ok20/view/common-info.html?regNumber=0830500000225003923</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300034525000086</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>№ 0830500000225003930</t>
+          <t>№ 0330300016625000093</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ СТАНЦИЯ СКОРОЙ МЕДИЦИНСКОЙ ПОМОЩИ" ИМЕНИ Н.Л. ТУРУПАНОВА</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Поставка продуктов питания</t>
+          <t>Поставка изделий медицинского назначения (Шприц общего назначения )</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>966 625,00 ₽</t>
+          <t>454 570,00 ₽</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>20.10.2025, 17.11.2025, 07.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>44-ФЗ Открытый конкурс в электронной форме</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ok20/view/common-info.html?regNumber=0830500000225003930</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300016625000093</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>№ 0130100004525000087</t>
+          <t>№ 0330300054925000049</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>УПРАВЛЕНИЕ СУДЕБНОГО ДЕПАРТАМЕНТА В ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "КОМПЛЕКСНЫЙ ЦЕНТР СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ НАСЕЛЕНИЯ СОКОЛЬСКОГО РАЙОНА"</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Текущий ремонт здания Череповецкого городского суда Вологодской области</t>
+          <t>Продуктовые наборы</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>264 973,39 ₽</t>
+          <t>22 500,00 ₽</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,145 +688,145 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0130100004525000087</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300054925000049</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>№ 0830500000225003932</t>
+          <t>№ 0330200019125000045</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ПСИХОНЕВРОЛОГИЧЕСКИЙ ДИСПАНСЕР № 2"</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Поставка продуктов питания</t>
+          <t>Поставка основных средств (кресла офисные)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3 320 726,25 ₽</t>
+          <t>108 660,00 ₽</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>20.10.2025, 17.11.2025, 07.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>44-ФЗ Открытый конкурс в электронной форме</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ok20/view/common-info.html?regNumber=0830500000225003932</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200019125000045</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>№ 0830500000225003921</t>
+          <t>№ 0330300190725000011</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "КОМПЛЕКСНЫЙ ЦЕНТР СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ НАСЕЛЕНИЯ НЮКСЕНСКОГО РАЙОНА"</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Поставка продуктов питания</t>
+          <t>Поставка офисной мебели</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2 642 877,50 ₽</t>
+          <t>157 209,00 ₽</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>20.10.2025, 17.11.2025, 07.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>44-ФЗ Открытый конкурс в электронной форме</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ok20/view/common-info.html?regNumber=0830500000225003921</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300190725000011</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>№ 0830500000225004240</t>
+          <t>№ 0330300010325000397</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА № 2"</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Поставка средств автотранспортных</t>
+          <t>Поставка лекарственного препарата для медицинского применения (ЭСМОЛОЛ)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3 330 000,00 ₽</t>
+          <t>12 165,00 ₽</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004240</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300010325000397</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>№ 0130100000425000026</t>
+          <t>№ 0330300051225000204</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>УПРАВЛЕНИЕ ФЕДЕРАЛЬНОЙ НАЛОГОВОЙ СЛУЖБЫ ПО ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "ЦЕНТРАЛИЗОВАННАЯ БУХГАЛТЕРИЯ, ОБСЛУЖИВАЮЩАЯ МУНИЦИПАЛЬНЫЕ УЧРЕЖДЕНИЯ ГОРОДА ВОЛОГДЫ"</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>На оказание услуг по пультовой охране и тревожной сигнализации объектов Управления Федеральной налоговой службы по Вологодской области</t>
+          <t>Оказание услуг по открытию возобновляемой кредитной линии в кредитной организации с лимитом задолженности в размере 100 000 000 (Сто миллионов) рублей в рамках исполнения бюджета города Вологды</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>901 703,40 ₽</t>
+          <t>20 670 000,00 ₽</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>23.10.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -836,177 +836,177 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0130100000425000026</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0330300051225000204</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>№ 0830500000225004239</t>
+          <t>№ 0330500001125000460</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ДЕТСКАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА"</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Оказание услуг по добровольному страхованию от несчастных случаев и болезней</t>
+          <t>Поставка лекарственного препарата для медицинского применения Эзомепразол</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1 308 232,17 ₽</t>
+          <t>32 192,01 ₽</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>, , 17.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004239</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330500001125000460</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>№ 0330300051925000194</t>
+          <t>№ 0330500001125000459</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОГО МУНИЦИПАЛЬНОГО ОКРУГА "РАСЧЕТНО-АНАЛИТИЧЕСКИЙ ЦЕНТР"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ДЕТСКАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА"</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Поставка песка</t>
+          <t>Оказание услуг по обязательному страхованию гражданской ответственности владельцев транспортных средств</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>998 750,00 ₽</t>
+          <t>287 250,67 ₽</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0330300051925000194</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330500001125000459</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>№ 0330300005825000032</t>
+          <t>№ 0130600039525000061</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ХАРОВСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>АДМИНИСТРАЦИЯ ВОЖЕГОДСКОГО МУНИЦИПАЛЬНОГО ОКРУГА ВОЛОГОДСКОЙ ОБЛАСТИ</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Выполнение работ по монтажу пандуса по адресу: Вологодская обл, Харовский м.о., Погост Никольский с, Центральная ул, дом 4 (Пустораменский ФАП)</t>
+          <t>Выполнение работ по сносу аварийных домов, расположенных на территории Вожегодского муниципального округа</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>106 945,82 ₽</t>
+          <t>763 466,44 ₽</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>05.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>44-ФЗ Запрос котировок в электронной форме</t>
+          <t>44-ФЗ Электронный аукцион</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300005825000032</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0130600039525000061</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>№ 0830500000225004217</t>
+          <t>№ 0330300001625000034</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ЧЕРЕПОВЕЦКИЙ ГОРОДСКОЙ РОДИЛЬНЫЙ ДОМ"</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению региональной системы межведомственного электронного взаимодействия Вологодской области</t>
+          <t>Поставка лекарственного препарата для медицинского применения Окситоцин</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4 288 079,00 ₽</t>
+          <t>32 760,00 ₽</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004217</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300001625000034</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>№ 0330300005825000033</t>
+          <t>№ 0330200019425000055</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ХАРОВСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ПО ОБЕСПЕЧЕНИЮ СОДЕРЖАНИЯ И ЭКСПЛУАТАЦИИ НЕДВИЖИМОГО ИМУЩЕСТВА ВОЛОГОДСКОЙ ОБЛАСТИ "УПРАВЛЕНИЕ ПО ЭКСПЛУАТАЦИИ ЗДАНИЙ"</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Выполнение работ по монтажу пандуса по адресу: Вологодская обл, Харовский м.о., Поповка д, дом 5 (Азлецкий ФАП)</t>
+          <t>Поставка антигололедных материалов</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>214 207,88 ₽</t>
+          <t>177 329,00 ₽</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1021,34 +1021,34 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300005825000033</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200019425000055</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>№ 0330300005825000034</t>
+          <t>№ 0330200019725000048</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ХАРОВСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "БЮРО СУДЕБНО-МЕДИЦИНСКОЙ ЭКСПЕРТИЗЫ"</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Выполнение работ по монтажу пандуса по адресу: Вологодская обл, Харовский м.о., Кумзеро с, дом 5 (Кумзерский ФАП)</t>
+          <t>Поставка филамента для газового хроматографа</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>183 104,38 ₽</t>
+          <t>77 067,34 ₽</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1058,34 +1058,34 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300005825000034</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200019725000048</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>№ 0330300005825000035</t>
+          <t>№ 0330200016225000073</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ХАРОВСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ НАРКОЛОГИЧЕСКИЙ ДИСПАНСЕР № 1"</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Выполнение работ по монтажу пандуса по адресу: Вологодская обл, Харовский м.о., Разинское с/п, Гора д, дом 65 (Разинский ФАП)</t>
+          <t>Поставка реагентов к биохимическому анализатору «Вита Лайн 200» (1)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>191 912,96 ₽</t>
+          <t>17 530,16 ₽</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1095,71 +1095,71 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300005825000035</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200016225000073</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>№ 0830500000225004218</t>
+          <t>№ 0330200016825000310</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА"</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению информационной системы, предназначенной для оказания массовых социально значимых услуг в электронном виде</t>
+          <t>Поставка лекарственного препарата для медицинского применения Спиронолактон</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5 364 453,50 ₽</t>
+          <t>76 800,00 ₽</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>01.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004218</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200016825000310</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>№ 0330300005825000036</t>
+          <t>№ 0330200016825000312</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ХАРОВСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА"</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Выполнение работ по монтажу пандуса по адресу: Вологодская обл, Харовский м.о., Золотава д, дом 13 (Фроловский ФАП)</t>
+          <t>Поставка лекарственного препарата для медицинского применения ВАЛЬПРОЕВАЯ КИСЛОТА</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>226 863,50 ₽</t>
+          <t>72 390,00 ₽</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>01.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1169,14 +1169,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300005825000036</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200016825000312</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>№ 0830500000225004220</t>
+          <t>№ 0830500000225004236</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1186,12 +1186,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению государственной информационной системы "Общий реестр граждан, имеющих право на бесплатное предоставление земельных участков на территории Вологодской области"</t>
+          <t>Выполнение работ по изготовлению представительской (сувенирной) продукции</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1 860 012,00 ₽</t>
+          <t>3 200 000,00 ₽</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1206,14 +1206,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004220</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004236</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>№ 0830500000225004219</t>
+          <t>№ 0830500000225004262</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1223,54 +1223,54 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению государственной информационной системы Вологодской области «Автоматизированная система исполнения запросов».</t>
+          <t>Поставка программного обеспечения</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2 766 298,00 ₽</t>
+          <t>7 972 380,00 ₽</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004219</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830500000225004262</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>№ 0330200010125000075</t>
+          <t>№ 0330300051225000219</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ПСИХОНЕВРОЛОГИЧЕСКИЙ ДИСПАНСЕР № 1"</t>
+          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "ЦЕНТРАЛИЗОВАННАЯ БУХГАЛТЕРИЯ, ОБСЛУЖИВАЮЩАЯ МУНИЦИПАЛЬНЫЕ УЧРЕЖДЕНИЯ ГОРОДА ВОЛОГДЫ"</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Поставка лекарственного препарата для медицинского применения Бромдигидрохлорфенилбензодиазепин</t>
+          <t>Поставка бумаги для офисной техники</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>71 149,20 ₽</t>
+          <t>35 533,10 ₽</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1280,66 +1280,66 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200010125000075</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300051225000219</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>№ 0830500000225004225</t>
+          <t>№ 0330200000525000148</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ОНКОЛОГИЧЕСКИЙ ДИСПАНСЕР"</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению государственной информационной системы «Портал государственных и муниципальных услуг (функций) Вологодской области»</t>
+          <t>Поставка медицинских изделий (шприцев общего назначения)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2 509 056,00 ₽</t>
+          <t>300 160,00 ₽</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004225</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200000525000148</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>№ 0330200014525000089</t>
+          <t>№ 0330300051225000220</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ПСИХИАТРИЧЕСКАЯ БОЛЬНИЦА"</t>
+          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "ЦЕНТРАЛИЗОВАННАЯ БУХГАЛТЕРИЯ, ОБСЛУЖИВАЮЩАЯ МУНИЦИПАЛЬНЫЕ УЧРЕЖДЕНИЯ ГОРОДА ВОЛОГДЫ"</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Оказание услуг по проведению поверки средств измерений</t>
+          <t>Выполнение работ по изготовлению представительской (сувенирной) продукции</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>67 949,00 ₽</t>
+          <t>639 958,40 ₽</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1354,88 +1354,88 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200014525000089</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300051225000220</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>№ 0130100007725000055</t>
+          <t>№ 0330200010125000074</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>УПРАВЛЕНИЕ ФЕДЕРАЛЬНОЙ СЛУЖБЫ ПО НАДЗОРУ В СФЕРЕ ЗАЩИТЫ ПРАВ ПОТРЕБИТЕЛЕЙ И БЛАГОПОЛУЧИЯ ЧЕЛОВЕКА ПО ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ПСИХОНЕВРОЛОГИЧЕСКИЙ ДИСПАНСЕР № 1"</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Поставка (отпуск) нефтепродуктов через АЗС по топливным картам</t>
+          <t>Оказание медицинских услуг по проведению лабораторных исследований на 2026 год</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>779 300,00 ₽</t>
+          <t>456 025,00 ₽</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0130100007725000055</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200010125000074</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>№ 0330300061125000016</t>
+          <t>№ 0830500000225004238</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "КОМПЛЕКСНЫЙ ЦЕНТР СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ НАСЕЛЕНИЯ ХАРОВСКОГО РАЙОНА"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Поставка спец. одежды и обуви</t>
+          <t>Оказание услуг по предпочтовой подготовке и доставке (возврату) внутрироссийских и международных почтовых отправлений, направляемых в форме электронного документа или на бумажном носителе</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>161 396,71 ₽</t>
+          <t>2 300 000,00 ₽</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>44-ФЗ Запрос котировок в электронной форме</t>
+          <t>44-ФЗ Электронный аукцион</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300061125000016</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004238</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>№ 0830500000225004221</t>
+          <t>№ 0830500000225004231</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1445,12 +1445,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению государственной информационной системы обеспечения градостроительной деятельности Вологодской области с функциями автоматизированной информационно-аналитической поддержки осуществления полномочий в области градостроительной деятельности</t>
+          <t>Оказание услуг по комплексной уборке и содержанию территории БУЗ ВО «Вологодская областная инфекционная больница»</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2 709 000,00 ₽</t>
+          <t>3 360 693,60 ₽</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1465,71 +1465,71 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004221</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004231</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>№ 0830500000225004222</t>
+          <t>№ 0330300010325000394</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА № 2"</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению государственной информационной системы "Информационно-аналитическая система Ситуационного центра Губернатора Вологодской области"</t>
+          <t>Поставка лекарственного препарата для медицинского применения (ТЕХНЕЦИЙ [99MTС])</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3 144 000,00 ₽</t>
+          <t>84 040,00 ₽</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>05.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004222</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300010325000394</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>№ 0830500000225004224</t>
+          <t>№ 0130100007725000054</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>УПРАВЛЕНИЕ ФЕДЕРАЛЬНОЙ СЛУЖБЫ ПО НАДЗОРУ В СФЕРЕ ЗАЩИТЫ ПРАВ ПОТРЕБИТЕЛЕЙ И БЛАГОПОЛУЧИЯ ЧЕЛОВЕКА ПО ВОЛОГОДСКОЙ ОБЛАСТИ</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению автоматизированной информационной системы учета и регистрации тракторов, самоходных машин и прицепов к ним «Гостехнадзор Эксперт»</t>
+          <t>Техническое обслуживание кондиционеров</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>432 747,00 ₽</t>
+          <t>31 700,00 ₽</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1539,66 +1539,66 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004224</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0130100007725000054</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>№ 0830500000225004228</t>
+          <t>№ 0330300010325000395</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ КЛИНИЧЕСКАЯ БОЛЬНИЦА № 2"</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Оказание услуг по сопровождению, технической поддержке и сервисному обслуживанию автоматизированных систем службы занятости Вологодской области</t>
+          <t>Поставка лекарственного препарата для медицинского применения (ТЕХНЕЦИЯ [99MТС] МЕРТИАТИД)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3 707 000,00 ₽</t>
+          <t>51 921,00 ₽</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004228</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300010325000395</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>№ 0330300007625000320</t>
+          <t>№ 0130600048625000046</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ БОЛЬНИЦА № 3"</t>
+          <t>АДМИНИСТРАЦИЯ ВАШКИНСКОГО МУНИЦИПАЛЬНОГО ОКРУГА ВОЛОГОДСКОЙ ОБЛАСТИ</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Поставка глюкозы ИВД, реагента</t>
+          <t>Обустройство источников наружного противопожарного водоснабжения (разворотные площадки)</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>147 840,00 ₽</t>
+          <t>840 214,45 ₽</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1613,71 +1613,71 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300007625000320</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0130600048625000046</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>№ 0830500000225003879</t>
+          <t>№ 0330200000525000147</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ОНКОЛОГИЧЕСКИЙ ДИСПАНСЕР"</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Оказание услуг по организации общественного питания пациентов</t>
+          <t>Поставка салфеток нетканых в рулоне</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>9 255 000,00 ₽</t>
+          <t>499 200,00 ₽</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>16.10.2025, 17.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>44-ФЗ Открытый конкурс в электронной форме</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ok20/view/common-info.html?regNumber=0830500000225003879</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200000525000147</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>№ 0330200023525000045</t>
+          <t>№ 0830300002325000195</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ПРОТИВОТУБЕРКУЛЕЗНЫЙ ДИСПАНСЕР"</t>
+          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "СПЕЦАВТОТРАНС"</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Поставка строительных материалов (2)</t>
+          <t>Запасные части для коммунально-уборочной техники (модуль силового блока)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>71 223,53 ₽</t>
+          <t>167 940,00 ₽</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1687,34 +1687,34 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200023525000045</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830300002325000195</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>№ 0330200023525000046</t>
+          <t>№ 0830500000225004246</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ПРОТИВОТУБЕРКУЛЕЗНЫЙ ДИСПАНСЕР"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Оказание услуг по проведению прижизненных патолого-анатомических исследований биопсийного (операционного) материала_2026</t>
+          <t>Выполнение работ по техническому и аварийно-техническому обслуживанию лифтов</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>136 266,65 ₽</t>
+          <t>790 272,00 ₽</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1724,29 +1724,29 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200023525000046</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830500000225004246</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>№ 0330500000825000075</t>
+          <t>№ 0330200014125000027</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ЧЕРЕПОВЕЦКАЯ ДЕТСКАЯ ГОРОДСКАЯ ПОЛИКЛИНИКА № 1"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОГНЕМСКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Поставка реагентов для анализатора Mindray BС (3)</t>
+          <t>Оказание услуг по проведению лабораторных исследований на маркеры вирусных гепатитов В и С</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>287 622,00 ₽</t>
+          <t>19 212,82 ₽</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1761,29 +1761,29 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330500000825000075</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200014125000027</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>№ 0330300061125000015</t>
+          <t>№ 0830100001525000048</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "КОМПЛЕКСНЫЙ ЦЕНТР СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ НАСЕЛЕНИЯ ХАРОВСКОГО РАЙОНА"</t>
+          <t>ФЕДЕРАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ "МЕДИКО-САНИТАРНАЯ ЧАСТЬ № 35 ФЕДЕРАЛЬНОЙ СЛУЖБЫ ИСПОЛНЕНИЯ НАКАЗАНИЙ"</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Поставка столов трапеции</t>
+          <t>Поставка лекарственных препаратов для медицинского применения</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>38 352,00 ₽</t>
+          <t>50 145,00 ₽</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1798,29 +1798,29 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300061125000015</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830100001525000048</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>№ 0230100000225000299</t>
+          <t>№ 0330200014125000026</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ОТДЕЛЕНИЕ ФОНДА ПЕНСИОННОГО И СОЦИАЛЬНОГО СТРАХОВАНИЯ РОССИЙСКОЙ ФЕДЕРАЦИИ ПО ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОГНЕМСКИЙ ДОМ СОЦИАЛЬНОГО ОБСЛУЖИВАНИЯ"</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Поставка подгузников для взрослых (размер XS) в целях социального обеспечения граждан в 2025 году</t>
+          <t>Поставка спецодежды</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>618 685,20 ₽</t>
+          <t>199 416,57 ₽</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1835,182 +1835,182 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0230100000225000299</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200014125000026</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>№ 0830500000225004091</t>
+          <t>№ 0330200019725000047</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "БЮРО СУДЕБНО-МЕДИЦИНСКОЙ ЭКСПЕРТИЗЫ"</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Оказание охранных услуг</t>
+          <t>Поставка расходных материалов для газового хроматографа</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>6 594 854,40 ₽</t>
+          <t>453 377,02 ₽</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>29.10.2025, 17.11.2025, 14.11.2025</t>
+          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>44-ФЗ Открытый конкурс в электронной форме</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ok20/view/common-info.html?regNumber=0830500000225004091</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200019725000047</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>№ 0830300002325000196</t>
+          <t>№ 0830500000225004178</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "СПЕЦАВТОТРАНС"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Электротехнические материалы (зажимы ответвительные)</t>
+          <t>Приобретение в специализированный жилищный фонд области благоустроенной квартиры в г. Череповце Вологодской области для обеспечения жилыми помещениями детей-сирот, детей, оставшихся без попечения родителей, лиц из числа детей-сирот и детей, оставшихся без попечения родителей, не реализовавших право на обеспечение жилыми помещениями</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>324 750,00 ₽</t>
+          <t>3 085 000,00 ₽</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>01.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>44-ФЗ Запрос котировок в электронной форме</t>
+          <t>44-ФЗ Электронный аукцион</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830300002325000196</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004178</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>№ 0230100000225000298</t>
+          <t>№ 0830500000225004205</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ОТДЕЛЕНИЕ ФОНДА ПЕНСИОННОГО И СОЦИАЛЬНОГО СТРАХОВАНИЯ РОССИЙСКОЙ ФЕДЕРАЦИИ ПО ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Поставка Брайлевских дисплеев в целях социального обеспечения граждан в 2025 году</t>
+          <t>Поставка расходных материалов для клинико-диагностической лаборатории (Группы крови) (3)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>870 333,34 ₽</t>
+          <t>572 075,46 ₽</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>05.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>44-ФЗ Запрос котировок в электронной форме</t>
+          <t>44-ФЗ Электронный аукцион</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0230100000225000298</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004205</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>№ 0330200000625000082</t>
+          <t>№ 0830500000225004174</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ОФТАЛЬМОЛОГИЧЕСКАЯ БОЛЬНИЦА"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Поставка лекарственных препаратов для медицинского применения</t>
+          <t>Приобретение в специализированный жилищный фонд области благоустроенной квартиры в г. Череповце Вологодской области для обеспечения жилыми помещениями детей-сирот, детей, оставшихся без попечения родителей, лиц из числа детей-сирот и детей, оставшихся без попечения родителей, не реализовавших право на обеспечение жилыми помещениями</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>230 414,50 ₽</t>
+          <t>3 085 000,00 ₽</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">10.11.2025, 17.11.2025, </t>
+          <t>01.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>44-ФЗ Запрос котировок в электронной форме</t>
+          <t>44-ФЗ Электронный аукцион</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200000625000082</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004174</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>№ 0330500000925000046</t>
+          <t>№ 0330200010925000063</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ЧЕРЕПОВЕЦКАЯ ДЕТСКАЯ ГОРОДСКАЯ ПОЛИКЛИНИКА № 3"</t>
+          <t>КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАНЯТОСТИ НАСЕЛЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Оказание услуг по техническому обслуживанию систем вентиляции и кондиционирования в 2026 году</t>
+          <t>Оказание услуг частной охраны (Охранный (технический) мониторинг)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>204 000,00 ₽</t>
+          <t>435 920,40 ₽</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2020,34 +2020,34 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330500000925000046</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200010925000063</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>№ 0830300002325000195</t>
+          <t>№ 0330200011325000028</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>МУНИЦИПАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "СПЕЦАВТОТРАНС"</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКИЙ ОБЛАСТНОЙ ПРОТИВОТУБЕРКУЛЕЗНЫЙ ДИСПАНСЕР № 2"</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Запасные части для коммунально-уборочной техники (модуль силового блока)</t>
+          <t>Выполнение работ по текущему ремонту системы рентгеновской диагностической стационарной общего назначения, цифровой РЕНЕКС-РЦ, установленной у Заказчика, без замены запасных частей и расходных материалов</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>167 940,00 ₽</t>
+          <t>100 666,67 ₽</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>10.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2057,34 +2057,34 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830300002325000195</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330200011325000028</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>№ 0130600031925000050</t>
+          <t>№ 0330100012525000097</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ФИНАНСОВОЕ УПРАВЛЕНИЕ АДМИНИСТРАЦИИ ЧАГОДОЩЕНСКОГО МУНИЦИПАЛЬНОГО ОКРУГА ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>ФЕДЕРАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "ИСПРАВИТЕЛЬНАЯ КОЛОНИЯ № 2 УПРАВЛЕНИЯ ФЕДЕРАЛЬНОЙ СЛУЖБЫ ИСПОЛНЕНИЯ НАКАЗАНИЙ ПО ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Поставка автомобильного бензина и дизельного топлива через АЗС с использованием топливных карт</t>
+          <t>оказание услуг по капитальному ремонту кабинета начальника отряда для нужд ФКУ ИК-2 УФСИН России пор Вологодской области в соответствии с техническим заданием</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>271 027,00 ₽</t>
+          <t>128 500,00 ₽</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2094,71 +2094,71 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0130600031925000050</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0330100012525000097</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>№ 0330300002625000201</t>
+          <t>№ 0830500000225004197</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ ДЕТСКАЯ БОЛЬНИЦА № 2"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Оказание услуг по изготовлению и поставке экстемпоральных форм лекарственных препаратов (растворы)</t>
+          <t>Услуги по санаторно-курортному лечению детей, проживающих на территории Вологодской области, по различным группам нозологий: педиатрия, гастроэнтерология, неврология, офтальмология, пульмонология, травматология и ортопедия, эндокринология, кардиология, оториноларингология (за исключением кохлеарной имплантации), урология. Услуги предоставляются по путевкам.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>492 700,00 ₽</t>
+          <t>3 805 200,00 ₽</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>05.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>44-ФЗ Запрос котировок в электронной форме</t>
+          <t>44-ФЗ Электронный аукцион</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300002625000201</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004197</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>№ 0330100010525000058</t>
+          <t>№ 0830500000225004229</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ФЕДЕРАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "УПРАВЛЕНИЕ АВТОМОБИЛЬНОЙ МАГИСТРАЛИ МОСКВА-АРХАНГЕЛЬСК ФЕДЕРАЛЬНОГО ДОРОЖНОГО АГЕНТСТВА"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Специализированное гидрометеорологическое обслуживание автомобильных дорог общего пользования федерального значения, находящихся в оперативном управлении ФКУ Упрдор "Холмогоры"</t>
+          <t>Оказание услуг радиотелефонной (сотовой) связи</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1 813 603,00 ₽</t>
+          <t>2 450 000,00 ₽</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2168,34 +2168,34 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0330100010525000058</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004229</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>№ 0330100012525000097</t>
+          <t>№ 0830500000225004232</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ФЕДЕРАЛЬНОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ "ИСПРАВИТЕЛЬНАЯ КОЛОНИЯ № 2 УПРАВЛЕНИЯ ФЕДЕРАЛЬНОЙ СЛУЖБЫ ИСПОЛНЕНИЯ НАКАЗАНИЙ ПО ВОЛОГОДСКОЙ ОБЛАСТИ"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>оказание услуг по капитальному ремонту кабинета начальника отряда для нужд ФКУ ИК-2 УФСИН России пор Вологодской области в соответствии с техническим заданием</t>
+          <t>Оказание услуг по предоставлению виртуальных выделенных каналов Ethernet (стационарные каналы связи)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>128 500,00 ₽</t>
+          <t>2 599 393,32 ₽</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2205,51 +2205,51 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0330100012525000097</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0830500000225004232</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>№ 0130600031225000392</t>
+          <t>№ 0330300007625000319</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>АДМИНИСТРАЦИЯ ВЕЛИКОУСТЮГСКОГО МУНИЦИПАЛЬНОГО ОКРУГА ВОЛОГОДСКОЙ ОБЛАСТИ</t>
+          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ВОЛОГОДСКАЯ ОБЛАСТНАЯ БОЛЬНИЦА № 3"</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Выполнение работ по зимнему содержанию автомобильных дорог общего пользования местного значения</t>
+          <t>Поставка лекарственного препарата для медицинского применения декстроза или отсутствие МНН</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1 010 000,00 ₽</t>
+          <t>493 000,00 ₽</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 17.11.2025</t>
+          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>44-ФЗ Электронный аукцион</t>
+          <t>44-ФЗ Запрос котировок в электронной форме</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/ea20/view/common-info.html?regNumber=0130600031225000392</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300007625000319</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>№ 0830500000225004249</t>
+          <t>№ 0830500000225004234</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2259,17 +2259,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Текущий ремонт лестничных маршей в здании учебного корпуса по адресу г. Вологда, ул. Чернышевского, д. 53</t>
+          <t>Оказание услуг по предоставлению прав (простых (неисключительных) лицензий) на использование обновлений специализированного программного обеспечения ViPNet Client , имеющегося у Заказчика.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1 585 138,11 ₽</t>
+          <t>448 995,00 ₽</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>07.11.2025, 17.11.2025, 14.11.2025</t>
+          <t>06.11.2025, 17.11.2025, 13.11.2025</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2279,29 +2279,29 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830500000225004249</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830500000225004234</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>№ 0330300005825000037</t>
+          <t>№ 0830500000225004261</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>БЮДЖЕТНОЕ УЧРЕЖДЕНИЕ ЗДРАВООХРАНЕНИЯ ВОЛОГОДСКОЙ ОБЛАСТИ "ХАРОВСКАЯ ЦЕНТРАЛЬНАЯ РАЙОННАЯ БОЛЬНИЦА"</t>
+          <t>ГОСУДАРСТВЕННОЕ КАЗЕННОЕ УЧРЕЖДЕНИЕ ВОЛОГОДСКОЙ ОБЛАСТИ "ЦЕНТР ЗАКУПОК"</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Выполнение работ по монтажу пандуса по адресу: Вологодская обл, Харовский м.о., Никулинское с, дом 13 (Шевницкий ФАП)</t>
+          <t>Оказание информационных услуг по продлению доступа по сети Интернет к ранее установленной базе данных нормативных и технических документов «Техэксперт: Лаборатория. Инспекция. Сертификация»</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>106 945,82 ₽</t>
+          <t>367 983,00 ₽</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0330300005825000037</t>
+          <t>https://zakupki.gov.ru/epz/order/notice/zk20/view/common-info.html?regNumber=0830500000225004261</t>
         </is>
       </c>
     </row>

</xml_diff>